<commit_message>
Done: Schedule Appointment, Reschedule Appointment, Cancel Appointment, View Scheduled Appointment
</commit_message>
<xml_diff>
--- a/data/AppointmentList.xlsx
+++ b/data/AppointmentList.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2dc85ffdfb189c0/Desktop/School Projects/SC2002 - OBJECT ORIENTIATED DESIGN ^0 PROGRAMMING/OOP_Proj/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="45" documentId="11_F25DC773A252ABDACC104886B99A6D005BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E9B5BA6-57C0-4202-9037-886C5D21E9EB}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="11_F25DC773A252ABDACC104886B99A6D005BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E990D5B-A462-44A0-92C1-FFABB91B6834}"/>
   <bookViews>
-    <workbookView xWindow="47895" yWindow="0" windowWidth="19410" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29400" yWindow="480" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
   <si>
     <t>Appointment ID</t>
   </si>
@@ -78,9 +78,6 @@
     <t>H002</t>
   </si>
   <si>
-    <t>Approved</t>
-  </si>
-  <si>
     <t>OR003</t>
   </si>
   <si>
@@ -88,12 +85,22 @@
   </si>
   <si>
     <t>2024-11-17T09:43:21.814164</t>
+  </si>
+  <si>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Available</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -166,10 +173,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -438,18 +441,18 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="28.81640625" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="20.81640625" customWidth="1"/>
-    <col min="7" max="7" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.453125"/>
+    <col min="2" max="2" customWidth="true" width="28.81640625"/>
+    <col min="3" max="3" customWidth="true" width="19.1796875"/>
+    <col min="4" max="4" customWidth="true" width="14.1796875"/>
+    <col min="5" max="5" customWidth="true" width="19.0"/>
+    <col min="6" max="6" customWidth="true" width="20.81640625"/>
+    <col min="7" max="7" customWidth="true" width="20.6328125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -473,63 +476,63 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="C2" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="E2" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s" s="0">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s" s="0">
         <v>17</v>
-      </c>
-      <c r="F4" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Done: View Past Appointment Outcome Records
</commit_message>
<xml_diff>
--- a/data/AppointmentList.xlsx
+++ b/data/AppointmentList.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2dc85ffdfb189c0/Desktop/School Projects/SC2002 - OBJECT ORIENTIATED DESIGN ^0 PROGRAMMING/OOP_Proj/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="57" documentId="11_F25DC773A252ABDACC104886B99A6D005BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E990D5B-A462-44A0-92C1-FFABB91B6834}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="11_F25DC773A252ABDACC104886B99A6D005BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C51542D7-87BD-4145-BAED-DED7C9BF7607}"/>
   <bookViews>
-    <workbookView xWindow="29400" yWindow="480" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30930" yWindow="2010" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Appointment ID</t>
   </si>
@@ -57,9 +57,6 @@
     <t>H005</t>
   </si>
   <si>
-    <t>Pending</t>
-  </si>
-  <si>
     <t>OR001</t>
   </si>
   <si>
@@ -94,13 +91,15 @@
   </si>
   <si>
     <t>Available</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -173,6 +172,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -446,13 +449,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.453125"/>
-    <col min="2" max="2" customWidth="true" width="28.81640625"/>
-    <col min="3" max="3" customWidth="true" width="19.1796875"/>
-    <col min="4" max="4" customWidth="true" width="14.1796875"/>
-    <col min="5" max="5" customWidth="true" width="19.0"/>
-    <col min="6" max="6" customWidth="true" width="20.81640625"/>
-    <col min="7" max="7" customWidth="true" width="20.6328125"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="28.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="20.81640625" customWidth="1"/>
+    <col min="7" max="7" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -476,63 +479,63 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="F2" t="s" s="0">
-        <v>11</v>
+      <c r="F2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s" s="0">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="C4" t="s" s="0">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
         <v>16</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix bugs on medical records
</commit_message>
<xml_diff>
--- a/data/AppointmentList.xlsx
+++ b/data/AppointmentList.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2dc85ffdfb189c0/Desktop/School Projects/SC2002 - OBJECT ORIENTIATED DESIGN ^0 PROGRAMMING/OOP_Proj/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="11_F25DC773A252ABDACC104886B99A6D005BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C51542D7-87BD-4145-BAED-DED7C9BF7607}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="11_F25DC773A252ABDACC104886B99A6D005BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C9B55FE-35B6-4763-A27F-0443EA4EE45E}"/>
   <bookViews>
     <workbookView xWindow="30930" yWindow="2010" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
   <si>
     <t>Appointment ID</t>
   </si>
@@ -94,12 +94,25 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>AP004</t>
+  </si>
+  <si>
+    <t>OR004</t>
+  </si>
+  <si>
+    <t>2024-11-19T19:10:12.981009</t>
+  </si>
+  <si>
+    <t>Pending</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -441,21 +454,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
-    <col min="2" max="2" width="28.81640625" customWidth="1"/>
-    <col min="3" max="3" width="19.1796875" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="20.81640625" customWidth="1"/>
-    <col min="7" max="7" width="20.6328125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="20.453125"/>
+    <col min="2" max="2" customWidth="true" width="28.81640625"/>
+    <col min="3" max="3" customWidth="true" width="19.1796875"/>
+    <col min="4" max="4" customWidth="true" width="14.1796875"/>
+    <col min="5" max="5" customWidth="true" width="19.0"/>
+    <col min="6" max="6" customWidth="true" width="20.81640625"/>
+    <col min="7" max="7" customWidth="true" width="20.6328125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -479,63 +492,83 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s" s="0">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
edited doctor's record appointment outcome
</commit_message>
<xml_diff>
--- a/data/AppointmentList.xlsx
+++ b/data/AppointmentList.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SC2001\OOP_Proj-1\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SC2001\OOP_Proj-2\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0ABF44D-365A-400A-BC7B-C450736A1E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62FD257F-2C77-4667-B663-FAEF5F45C634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Appointment ID</t>
   </si>
@@ -72,43 +72,49 @@
     <t>H025</t>
   </si>
   <si>
+    <t>OR003</t>
+  </si>
+  <si>
+    <t>2024-11-17T09:43:07.985412</t>
+  </si>
+  <si>
+    <t>2024-11-17T09:43:21.814164</t>
+  </si>
+  <si>
+    <t>Confirmed</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Available</t>
+  </si>
+  <si>
+    <t>OR004</t>
+  </si>
+  <si>
+    <t>AP004</t>
+  </si>
+  <si>
+    <t>AP005</t>
+  </si>
+  <si>
+    <t>2024-11-20T18:00</t>
+  </si>
+  <si>
+    <t>OR005</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Pending</t>
+  </si>
+  <si>
     <t>H002</t>
   </si>
   <si>
-    <t>OR003</t>
-  </si>
-  <si>
-    <t>2024-11-17T09:43:07.985412</t>
-  </si>
-  <si>
-    <t>2024-11-17T09:43:21.814164</t>
-  </si>
-  <si>
-    <t>Confirmed</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Available</t>
-  </si>
-  <si>
-    <t>Done</t>
-  </si>
-  <si>
-    <t>OR004</t>
-  </si>
-  <si>
-    <t>AP004</t>
-  </si>
-  <si>
-    <t>AP005</t>
-  </si>
-  <si>
-    <t>2024-11-20T18:00</t>
-  </si>
-  <si>
-    <t>OR005</t>
+    <t>Approved</t>
   </si>
 </sst>
 </file>
@@ -456,7 +462,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -498,13 +504,13 @@
         <v>7</v>
       </c>
       <c r="C2" t="s" s="0">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E2" t="s" s="0">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s" s="0">
         <v>10</v>
@@ -515,7 +521,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s" s="0">
         <v>9</v>
@@ -524,7 +530,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s" s="0">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s" s="0">
         <v>12</v>
@@ -535,27 +541,27 @@
         <v>13</v>
       </c>
       <c r="B4" t="s" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s" s="0">
         <v>14</v>
       </c>
       <c r="D4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="F4" t="s" s="0">
         <v>15</v>
-      </c>
-      <c r="E4" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="F4" t="s" s="0">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s" s="0">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s" s="0">
         <v>9</v>
@@ -564,30 +570,30 @@
         <v>8</v>
       </c>
       <c r="E5" t="s" s="0">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s" s="0">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s" s="0">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s" s="0">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s" s="0">
         <v>8</v>
       </c>
       <c r="E6" t="s" s="0">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s" s="0">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bugs for appointment outcome records
</commit_message>
<xml_diff>
--- a/data/AppointmentList.xlsx
+++ b/data/AppointmentList.xlsx
@@ -3,21 +3,21 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2dc85ffdfb189c0/Desktop/School Projects/SC2002 - OBJECT ORIENTIATED DESIGN ^0 PROGRAMMING/OOP_Proj/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="66" documentId="11_F25DC773A252ABDACC104886B99A6D005BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C9B55FE-35B6-4763-A27F-0443EA4EE45E}"/>
+  <xr:revisionPtr revIDLastSave="67" documentId="11_F25DC773A252ABDACC104886B99A6D005BDE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D33B4DD-5CCD-442C-B820-DEC421EA8D75}"/>
   <bookViews>
-    <workbookView xWindow="30930" yWindow="2010" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29370" yWindow="570" windowWidth="28800" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Appointment ID</t>
   </si>
@@ -93,9 +93,6 @@
     <t>Available</t>
   </si>
   <si>
-    <t>Done</t>
-  </si>
-  <si>
     <t>AP004</t>
   </si>
   <si>
@@ -105,14 +102,13 @@
     <t>2024-11-19T19:10:12.981009</t>
   </si>
   <si>
-    <t>Pending</t>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -185,10 +181,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -457,18 +449,18 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="20.453125"/>
-    <col min="2" max="2" customWidth="true" width="28.81640625"/>
-    <col min="3" max="3" customWidth="true" width="19.1796875"/>
-    <col min="4" max="4" customWidth="true" width="14.1796875"/>
-    <col min="5" max="5" customWidth="true" width="19.0"/>
-    <col min="6" max="6" customWidth="true" width="20.81640625"/>
-    <col min="7" max="7" customWidth="true" width="20.6328125"/>
+    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="2" max="2" width="28.81640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1796875" customWidth="1"/>
+    <col min="4" max="4" width="14.1796875" customWidth="1"/>
+    <col min="5" max="5" width="19" customWidth="1"/>
+    <col min="6" max="6" width="20.81640625" customWidth="1"/>
+    <col min="7" max="7" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -492,83 +484,83 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" t="s" s="0">
+      <c r="A2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s" s="0">
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s" s="0">
+      <c r="C2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s" s="0">
+      <c r="D2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s" s="0">
+      <c r="E2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s" s="0">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" t="s" s="0">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s" s="0">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s" s="0">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s" s="0">
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" t="s" s="0">
+      <c r="A4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" t="s" s="0">
+      <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" t="s" s="0">
+      <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" t="s" s="0">
+      <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" t="s" s="0">
+      <c r="E4" t="s">
         <v>19</v>
       </c>
-      <c r="F4" t="s" s="0">
+      <c r="F4" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" t="s" s="0">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
         <v>23</v>
-      </c>
-      <c r="B5" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s" s="0">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>